<commit_message>
Added tickets. Estimated time for tasks. Updated sprint backlog.
</commit_message>
<xml_diff>
--- a/BuildingInfo.xlsx
+++ b/BuildingInfo.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mochodek/Documents/Dydaktyka/Wyklady/IO/Laboratory classes/io-labs/08-sprint-planning/backlogs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF0AB65-F529-5940-B8B5-A280F6EFCF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C105F45-DDBC-4332-8311-78726AE2B04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="500" windowWidth="25600" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="500" windowWidth="25600" windowHeight="17500" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Opis" sheetId="3" r:id="rId1"/>
     <sheet name="Product Backlog" sheetId="1" r:id="rId2"/>
     <sheet name="Sprint Backlog #1" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,58 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
-  <si>
-    <t>Element rejestru produktu</t>
-  </si>
-  <si>
-    <t>Ważność</t>
-  </si>
-  <si>
-    <t>Pracochłonność</t>
-  </si>
-  <si>
-    <t>Kryteria akceptacji</t>
-  </si>
-  <si>
-    <t>Business Value (BV)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jako użytkownik mogę skorzystać z aplikacji za pomocą interfejsu użytkownika </t>
-  </si>
-  <si>
-    <t>Do późniejszej negocjacji</t>
-  </si>
-  <si>
-    <t>Zadania</t>
-  </si>
-  <si>
-    <t>Element przekopiowany z zakładki Rejestr Produktu</t>
-  </si>
-  <si>
-    <t>Zadanie nr 1 do elementu rejestru produktu</t>
-  </si>
-  <si>
-    <t>Zadanie nr 2 do elementu rejestru produktu</t>
-  </si>
-  <si>
-    <t>Zadanie nr 3 do elementu rejestru produktu</t>
-  </si>
-  <si>
-    <t>Zadanie nr 4 do elementu rejestru produktu</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pracochłonność </t>
-  </si>
-  <si>
-    <t>(dla elementu rejestru produktu)</t>
-  </si>
-  <si>
-    <t>(dla zadania)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t>Building Info</t>
   </si>
@@ -100,6 +58,21 @@
 </t>
   </si>
   <si>
+    <t>Element rejestru produktu</t>
+  </si>
+  <si>
+    <t>Ważność</t>
+  </si>
+  <si>
+    <t>Pracochłonność</t>
+  </si>
+  <si>
+    <t>Business Value (BV)</t>
+  </si>
+  <si>
+    <t>Kryteria akceptacji</t>
+  </si>
+  <si>
     <t>Jako twórca oprogramowania do zarządzania budynkami mogę korzystać z dostępnych funkcji zdalnie poprzez REST, aby móc  zintegrować narzędzie z moimi innymi aplikacjami</t>
   </si>
   <si>
@@ -154,14 +127,98 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">Jako użytkownik mogę skorzystać z aplikacji za pomocą interfejsu użytkownika </t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Do późniejszej negocjacji</t>
+  </si>
+  <si>
     <t>Cel Sprintu:</t>
+  </si>
+  <si>
+    <t>Zadania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pracochłonność </t>
+  </si>
+  <si>
+    <t>Nazwa ticketu - feature/1_addRest</t>
+  </si>
+  <si>
+    <t>w godzinach</t>
+  </si>
+  <si>
+    <t>1. Zapoznanie się z REST.</t>
+  </si>
+  <si>
+    <t>2. Dodanie REST do projektu.</t>
+  </si>
+  <si>
+    <t>3. Przetestowanie działania.</t>
+  </si>
+  <si>
+    <t>4. Implementacja struktur danych projektu.</t>
+  </si>
+  <si>
+    <t>Nazwa ticketu - feature/2_calcAreaFunctions</t>
+  </si>
+  <si>
+    <t>1. Dodanie metody - CalcArea do klasy abstrakcyjnej - Location.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Implementacja metody dla klasy - Room. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Implementacja metody dla klasy - Floor. </t>
+  </si>
+  <si>
+    <t>4. Implementacja metody dla klasy - Building.</t>
+  </si>
+  <si>
+    <t>Nazwa ticketu - feature/3_calcCubeFunctions</t>
+  </si>
+  <si>
+    <t>1. Dodanie metody - CalcCube do klasy abstrakcyjnej - Location.</t>
+  </si>
+  <si>
+    <t>2. Implementacja metody dla klasy - Room.</t>
+  </si>
+  <si>
+    <t>3. Implementacja metody dla klasy - Floor.</t>
+  </si>
+  <si>
+    <t>Nazwa ticketu - feature/4_calcHeatingFunctions</t>
+  </si>
+  <si>
+    <t>1. Dodanie metody - CalcHeating do klasy abstrakcyjnej - Location.</t>
+  </si>
+  <si>
+    <t>Nazwa ticketu - feature/5_calcEnergyFunctions</t>
+  </si>
+  <si>
+    <t>1. Dodanie metody - CalcEnergy do klasy abstrakcyjnej - Location.</t>
+  </si>
+  <si>
+    <t>Nazwa ticketu - feature/6_getInfoAboutSpecificRooms</t>
+  </si>
+  <si>
+    <t>1. Dodanie metody - GetHighEnergyRooms (float parameter) do klasy Building. Zwraca pomieszczenia.</t>
+  </si>
+  <si>
+    <t>Nazwa ticketu - feature/7_GUI</t>
+  </si>
+  <si>
+    <t>Do negocjacji</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -208,13 +265,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -247,7 +318,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -273,27 +344,38 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="Hiperłącze" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperłącze" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Odwiedzone hiperłącze" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -325,6 +407,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
@@ -365,7 +448,9 @@
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Element rejestru produktu" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ważność" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Pracochłonność" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Pracochłonność" dataDxfId="6">
+      <calculatedColumnFormula>SUM('Sprint Backlog #1'!C6:C9)</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Business Value (BV)" dataDxfId="5"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Kryteria akceptacji" dataDxfId="4"/>
   </tableColumns>
@@ -709,26 +794,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="95.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="24.95">
       <c r="A1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="84.95" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="204" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="189">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -746,125 +833,158 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="52" style="3" customWidth="1"/>
     <col min="2" max="2" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="20.100000000000001">
       <c r="A1" s="6" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="110.25">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4">
         <v>20</v>
       </c>
+      <c r="C2" s="11">
+        <f>SUM('Sprint Backlog #1'!C6:C9)</f>
+        <v>20</v>
+      </c>
       <c r="D2" s="4">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="84.95">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4">
         <v>15</v>
       </c>
+      <c r="C3" s="11">
+        <f>SUM('Sprint Backlog #1'!C12:C15)</f>
+        <v>8</v>
+      </c>
       <c r="D3" s="4">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="84.95">
       <c r="A4" s="3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4">
         <v>12</v>
       </c>
+      <c r="C4" s="11">
+        <f>SUM('Sprint Backlog #1'!C18:C21)</f>
+        <v>8</v>
+      </c>
       <c r="D4" s="4">
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="68.099999999999994">
       <c r="A5" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B5" s="4">
         <v>10</v>
       </c>
+      <c r="C5" s="11">
+        <f>SUM('Sprint Backlog #1'!C24:C27)</f>
+        <v>8</v>
+      </c>
       <c r="D5" s="4">
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="68.099999999999994">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4">
         <v>10</v>
       </c>
+      <c r="C6" s="11">
+        <f>SUM('Sprint Backlog #1'!C30:C33)</f>
+        <v>8</v>
+      </c>
       <c r="D6" s="4">
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="68.099999999999994">
       <c r="A7" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4">
         <v>10</v>
       </c>
+      <c r="C7" s="11">
+        <f>SUM('Sprint Backlog #1'!C36)</f>
+        <v>16</v>
+      </c>
       <c r="D7" s="4">
         <v>1.5</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="33.950000000000003">
       <c r="A8" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -883,86 +1003,296 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:C13"/>
+  <dimension ref="A2:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="45.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="48.83203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="45.125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="51.875" style="3" customWidth="1"/>
     <col min="3" max="3" width="33" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17.100000000000001">
       <c r="A2" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18.75">
+      <c r="A4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75">
+      <c r="A5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="66.75" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75">
+      <c r="B7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75">
+      <c r="B8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75">
+      <c r="B9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75"/>
+    <row r="11" spans="1:3" ht="15.75">
+      <c r="A11" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+    </row>
+    <row r="12" spans="1:3" ht="66" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75">
+      <c r="A13" s="10"/>
+      <c r="B13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75">
+      <c r="B14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75">
+      <c r="A15" s="10"/>
+      <c r="B15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75">
+      <c r="A16" s="10"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75">
+      <c r="A17" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+    </row>
+    <row r="18" spans="1:3" ht="63">
+      <c r="A18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75">
+      <c r="A19" s="10"/>
+      <c r="B19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75">
+      <c r="B20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75">
+      <c r="A21" s="10"/>
+      <c r="B21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75"/>
+    <row r="23" spans="1:3" ht="15.75">
+      <c r="A23" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+    </row>
+    <row r="24" spans="1:3" ht="47.25">
+      <c r="A24" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="B24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75">
+      <c r="A25" s="10"/>
+      <c r="B25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75">
+      <c r="B26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75">
+      <c r="A27" s="10"/>
+      <c r="B27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75"/>
+    <row r="29" spans="1:3" ht="15.75">
+      <c r="A29" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="13"/>
+    </row>
+    <row r="30" spans="1:3" ht="47.25">
+      <c r="A30" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="B10" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="B13" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
+      <c r="B30" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75">
+      <c r="A31" s="10"/>
+      <c r="B31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75">
+      <c r="B32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75">
+      <c r="A33" s="10"/>
+      <c r="B33" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75"/>
+    <row r="35" spans="1:3" ht="15.75">
+      <c r="A35" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="12"/>
+      <c r="C35" s="13"/>
+    </row>
+    <row r="36" spans="1:3" ht="78.75">
+      <c r="A36" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75">
+      <c r="A37" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="12"/>
+      <c r="C37" s="13"/>
+    </row>
+    <row r="38" spans="1:3" ht="31.5">
+      <c r="A38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
add new elements to product backlog
</commit_message>
<xml_diff>
--- a/BuildingInfo.xlsx
+++ b/BuildingInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mochodek/Documents/Dydaktyka/Wyklady/IO/Laboratory classes/io-labs/08-sprint-planning/backlogs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\IO2021\IO_2021_I8.2_Beta_BI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C105F45-DDBC-4332-8311-78726AE2B04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9DCA91-133F-4271-99F5-96F1F5CCD215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="500" windowWidth="25600" windowHeight="17500" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Opis" sheetId="3" r:id="rId1"/>
@@ -22,9 +22,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>Building Info</t>
   </si>
@@ -130,12 +128,6 @@
     <t xml:space="preserve">Jako użytkownik mogę skorzystać z aplikacji za pomocą interfejsu użytkownika </t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Do późniejszej negocjacji</t>
-  </si>
-  <si>
     <t>Cel Sprintu:</t>
   </si>
   <si>
@@ -212,13 +204,34 @@
   </si>
   <si>
     <t>Do negocjacji</t>
+  </si>
+  <si>
+    <t>Jako zarządca budynku mogę otrzymać informację o pomieszczeniach w budynku, które nie przekraczają określonego poziom oświetlenia / m^2 podany jako parametr, aby znaleźć miejsca do poprawy w infrastrukturze.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o Na wejściu oprócz struktury budynku podana wartość graniczna
+o Na wyjściu obiekty reprezentujące pomieszczenia nie przekraczające zadanej normy.
+</t>
+  </si>
+  <si>
+    <t>Jako zarządca budynku mogę otrzymać informację o wysokości podatku za powierzchnię mieszkaniową po podaniu na wejściu kosztu za metr kwadratowy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o Na wejściu oprócz pożadanego pomieszczenia podawana również wysokość podatku za 1 m^2
+o Na wyjściu wysokość podatku od danego mieszkania
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o Opisane okienka na wartości wejściowe takie jak id budynku, piętra, pomieszczenia itp.
+o Wylistowane opcje co można zrobić z danym obiektem.
+o Jeżeli wybrane zostało zapytanie to na wyświetli się okno z odpowiedzią. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -357,25 +370,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hiperłącze" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperłącze" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperłącze" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperłącze" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperłącze" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperłącze" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperłącze" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperłącze" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Odwiedzone hiperłącze" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Odwiedzone hiperłącze" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Odwiedzone hiperłącze" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Odwiedzone hiperłącze" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Odwiedzone hiperłącze" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Odwiedzone hiperłącze" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Odwiedzone hiperłącze" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Odwiedzone hiperłącze" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Odwiedzone hiperłącze" xfId="14" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -443,8 +456,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela2" displayName="Tabela2" ref="A1:E8" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A1:E8" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela2" displayName="Tabela2" ref="A1:E10" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A1:E10" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Element rejestru produktu" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ważność" dataDxfId="7"/>
@@ -798,22 +811,22 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="95.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="24.95">
+    <row r="1" spans="1:1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="84.95" customHeight="1">
+    <row r="2" spans="1:1" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="189">
+    <row r="4" spans="1:1" ht="189" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -830,13 +843,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52" style="3" customWidth="1"/>
     <col min="2" max="2" width="15" style="4" bestFit="1" customWidth="1"/>
@@ -845,7 +858,7 @@
     <col min="5" max="5" width="58.125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.100000000000001">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -862,7 +875,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="110.25">
+    <row r="2" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -880,7 +893,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="84.95">
+    <row r="3" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -898,7 +911,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="84.95">
+    <row r="4" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -916,7 +929,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="68.099999999999994">
+    <row r="5" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -934,7 +947,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="68.099999999999994">
+    <row r="6" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -952,7 +965,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="68.099999999999994">
+    <row r="7" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -970,21 +983,55 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="33.950000000000003">
+    <row r="8" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>21</v>
+      <c r="B8" s="4">
+        <v>20</v>
+      </c>
+      <c r="C8" s="11">
+        <v>20</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2.5</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>22</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="4">
+        <v>10</v>
+      </c>
+      <c r="C9" s="11">
+        <v>8</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="4">
+        <v>10</v>
+      </c>
+      <c r="C10" s="11">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1003,296 +1050,291 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:C39"/>
+  <dimension ref="A2:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="51.875" style="3" customWidth="1"/>
     <col min="3" max="3" width="33" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="17.100000000000001">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="18.75">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75">
-      <c r="A5" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="66.75" customHeight="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" s="11">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="11">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" s="11">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75"/>
-    <row r="11" spans="1:3" ht="15.75">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
     </row>
-    <row r="12" spans="1:3" ht="66" customHeight="1">
+    <row r="12" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C13" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C15" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
     </row>
-    <row r="17" spans="1:3" ht="15.75">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="13"/>
     </row>
-    <row r="18" spans="1:3" ht="63">
+    <row r="18" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C19" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C21" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75"/>
-    <row r="23" spans="1:3" ht="15.75">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="13"/>
     </row>
-    <row r="24" spans="1:3" ht="47.25">
+    <row r="24" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C24" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C25" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C26" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C27" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75"/>
-    <row r="29" spans="1:3" ht="15.75">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="13"/>
     </row>
-    <row r="30" spans="1:3" ht="47.25">
+    <row r="30" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C30" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C31" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C32" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C33" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75"/>
-    <row r="35" spans="1:3" ht="15.75">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B35" s="12"/>
       <c r="C35" s="13"/>
     </row>
-    <row r="36" spans="1:3" ht="78.75">
+    <row r="36" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C36" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="13"/>
     </row>
-    <row r="38" spans="1:3" ht="31.5">
+    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.75"/>
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>